<commit_message>
Updated jxls 3 report in demo
</commit_message>
<xml_diff>
--- a/src/art-parent/art/src/main/webapp/WEB-INF/work/templates/sample-jxls3.xlsx
+++ b/src/art-parent/art/src/main/webapp/WEB-INF/work/templates/sample-jxls3.xlsx
@@ -15,6 +15,64 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="B5")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="results" var="row" lastCell="B5")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
@@ -24,20 +82,20 @@
     <t>Volume</t>
   </si>
   <si>
-    <t>${results.VOLUME}</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
-    <t>${results.ITEM_NAME}</t>
+    <t>${row.ITEM_NAME}</t>
+  </si>
+  <si>
+    <t>${row.VOLUME}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +135,19 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -236,7 +307,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>${results.ITEM_NAME}</c:v>
+                  <c:v>${row.ITEM_NAME}</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -263,11 +334,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="210234368"/>
-        <c:axId val="210264832"/>
+        <c:axId val="46936448"/>
+        <c:axId val="46937984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210234368"/>
+        <c:axId val="46936448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -276,7 +347,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210264832"/>
+        <c:crossAx val="46937984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -284,7 +355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210264832"/>
+        <c:axId val="46937984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -295,7 +366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210234368"/>
+        <c:crossAx val="46936448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -649,11 +720,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +742,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -679,10 +750,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -755,8 +826,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>